<commit_message>
Fix ROCF DR Acc age adjustment
</commit_message>
<xml_diff>
--- a/data-raw/tables.xlsx
+++ b/data-raw/tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/GitHub/neuronorma/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E779EF8-8940-5D4E-9D1A-544573A1E40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE81429F-B79F-B34F-BFE1-74481F2A8B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Age" sheetId="1" r:id="rId1"/>
     <sheet name="Education" sheetId="2" r:id="rId2"/>
     <sheet name="TMTa &lt;50 Education" sheetId="4" r:id="rId3"/>
+    <sheet name="ROCF DR Acc &lt;50 Education" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="486">
   <si>
     <t>SS</t>
   </si>
@@ -4892,19 +4893,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD1ADC0-39C1-5146-853B-75F39D4F50C6}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="8" width="10.83203125" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="3" t="s">
         <v>197</v>
@@ -4917,12 +4919,11 @@
         <v>1</v>
       </c>
       <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s">
         <v>483</v>
       </c>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -4942,13 +4943,10 @@
         <v>484</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -4963,12 +4961,11 @@
       <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -4983,12 +4980,11 @@
       <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -5003,12 +4999,11 @@
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -5023,12 +5018,11 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -5043,12 +5037,11 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -5063,12 +5056,11 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -5083,12 +5075,11 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -5103,12 +5094,11 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -5128,13 +5118,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -5154,13 +5141,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -5182,11 +5166,8 @@
       <c r="G13" s="3">
         <v>0</v>
       </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -5208,11 +5189,8 @@
       <c r="G14" s="3">
         <v>0</v>
       </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -5234,11 +5212,8 @@
       <c r="G15" s="3">
         <v>0</v>
       </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -5258,13 +5233,10 @@
         <v>-1</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -5284,13 +5256,10 @@
         <v>-1</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -5310,13 +5279,10 @@
         <v>-1</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -5336,13 +5302,10 @@
         <v>-1</v>
       </c>
       <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -5364,11 +5327,8 @@
       <c r="G20" s="3">
         <v>-1</v>
       </c>
-      <c r="H20" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -5390,11 +5350,8 @@
       <c r="G21" s="3">
         <v>-1</v>
       </c>
-      <c r="H21" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -5416,11 +5373,8 @@
       <c r="G22" s="3">
         <v>-1</v>
       </c>
-      <c r="H22" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -5440,17 +5394,13 @@
         <v>-2</v>
       </c>
       <c r="G23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H23" s="3">
         <v>-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6927,4 +6877,1477 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E0E50C-EB2D-ED41-B514-307A514AACFA}">
+  <dimension ref="A1:AG15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AG30" sqref="AG30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="33" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+    </row>
+    <row r="2" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="2">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2">
+        <v>30</v>
+      </c>
+      <c r="O2" s="2">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2">
+        <v>34</v>
+      </c>
+      <c r="S2" s="2">
+        <v>35</v>
+      </c>
+      <c r="T2" s="2">
+        <v>36</v>
+      </c>
+      <c r="U2" s="2">
+        <v>37</v>
+      </c>
+      <c r="V2" s="2">
+        <v>38</v>
+      </c>
+      <c r="W2" s="2">
+        <v>39</v>
+      </c>
+      <c r="X2" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>46</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="R14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="S14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="T14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>0</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="R15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="S15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="T15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="U15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="V15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="W15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:AG1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>